<commit_message>
Finished all of Morgan's edits except for the suplicates issue.
</commit_message>
<xml_diff>
--- a/Output Data/Parameter_data.xlsx
+++ b/Output Data/Parameter_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A184"/>
+  <dimension ref="A1:A179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,42 +430,42 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Benz[a]anthracene</t>
+          <t>Benz[A]Anthracene</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Benzo[a]pyrene</t>
+          <t>Benzo[A]Pyrene</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Benzo[b]fluoranthene</t>
+          <t>Benzo[B]Fluoranthene</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Benzo[e]pyrene</t>
+          <t>Benzo[E]Pyrene</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Benzo[g,h,i]perylene</t>
+          <t>Benzo[G,H,I]Perylene</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Benzo[k]fluoranthene</t>
+          <t>Benzo[K]Fluoranthene</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C1-Fluoranthenes_Pyrenes</t>
+          <t>C1-Fluoranthenes_pyrenes</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>C1-Phenanthrenes_Anthracenes</t>
+          <t>C1-Phenanthrenes_anthracenes</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>C2-Fluoranthenes_Pyrenes</t>
+          <t>C2-Fluoranthenes_pyrenes</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>C2-Phenanthrenes_Anthracenes</t>
+          <t>C2-Phenanthrenes_anthracenes</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>C3-Fluoranthenes_Pyrenes</t>
+          <t>C3-Fluoranthenes_pyrenes</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>C3-Phenanthrenes_Anthracenes</t>
+          <t>C3-Phenanthrenes_anthracenes</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>C4-Phenanthrenes_Anthracenes</t>
+          <t>C4-Phenanthrenes_anthracenes</t>
         </is>
       </c>
     </row>
@@ -724,14 +724,14 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Cis_Trans Decalin</t>
+          <t>Cis_trans Decalin</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Dibenzo[a,h]anthracene</t>
+          <t>Dibenzo[A,H]Anthracene</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Indeno[1,2,3-c,d]pyrene</t>
+          <t>Indeno[1,2,3-C,D]Pyrene</t>
         </is>
       </c>
     </row>
@@ -808,21 +808,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>C1-Dibenzo[a,h]anthracene</t>
+          <t>C1-Dibenzo[A,H]Anthracene</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>C2-Dibenzo[a,h]anthracene</t>
+          <t>C2-Dibenzo[A,H]Anthracene</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>C3-Dibenzo[a,h]anthracene</t>
+          <t>C3-Dibenzo[A,H]Anthracene</t>
         </is>
       </c>
     </row>
@@ -906,63 +906,63 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Benzo(a)fluoranthene</t>
+          <t>Benzo[A]Fluoranthene</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Benzo(b)fluorene</t>
+          <t>Benzo[B]Fluorene</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>C20-TAS</t>
+          <t>C20-Tas</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>C21-TAS</t>
+          <t>C21-Tas</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>C26(20R)/C27(20S)-TAS</t>
+          <t>C26(20r)/C27(20s)-Tas</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>C26(20S)-TAS</t>
+          <t>C26(20s)-Tas</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>C27(20R)-TAS</t>
+          <t>C27(20r)-Tas</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>C28(20R)-TAS</t>
+          <t>C28(20r)-Tas</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>C28(20S)-TAS</t>
+          <t>C28(20s)-Tas</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>C4-Fluoranthenes_Pyrenes</t>
+          <t>C4-Fluoranthenes_pyrenes</t>
         </is>
       </c>
     </row>
@@ -1018,623 +1018,588 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Benzo(a)anthracene</t>
+          <t>Benzo[A]Anthracene</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Benzo(a)pyrene</t>
+          <t>C1-Benz[A]Anthracenes/Chrysenes</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Benzo(b)fluoranthene</t>
+          <t>C1-Fluoranthenes/Pyrenes</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Benzo(g,h,i)perylene</t>
+          <t>C1-Phenanthrenes/Anthracenes</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Benzo(k)fluoranthene</t>
+          <t>C2-Benz[A]Anthracenes/Chrysenes</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>C1-Benz(a)anthracenes/Chrysenes</t>
+          <t>C2-Phenanthrenes/Anthracenes</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>C1-Fluoranthenes/pyrenes</t>
+          <t>C3-Benz[A]Anthracenes/Chrysenes</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>C1-Phenanthrenes/anthracenes</t>
+          <t>C3-Phenanthrenes/Anthracenes</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>C2-Benz(a)anthracenes/Chrysenes</t>
+          <t>C4-Benz[A]Anthracenes/Chrysenes</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>C2-Phenanthrenes/anthracenes</t>
+          <t>C4-Phenanthrenes/Anthracenes</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>C3-Benz(a)anthracenes/Chrysenes</t>
+          <t>Dibenzo(A,H)Anthracene</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>C3-Phenanthrenes/anthracenes</t>
+          <t>Indeno(1,2,3-C,D)Pyrene</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>C4-Benz(a)anthracenes/Chrysenes</t>
+          <t>Pahs, Total (Db Calculated)</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>C4-Phenanthrenes/anthracenes</t>
+          <t>Pahs, Total High Molecular Weight Pahs (Db Calculated)</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Dibenzo(a,h)anthracene</t>
+          <t>Pahs, Total High Molecular Wt Pahs (Reported)</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Indeno(1,2,3-c,d)pyrene</t>
+          <t>Pahs, Total Low Molecular Weight Pahs (Db Calculated)</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>PAHs, total (DB calculated)</t>
+          <t>Pahs, Total Low Molecular Wt Pahs (Reported)</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>PAHs, total high molecular weight PAHs (DB calculated)</t>
+          <t>Cdfw-Ospr</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>PAHs, total high molecular wt PAHs (reported)</t>
+          <t>Epa Pah16</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>PAHs, total low molecular weight PAHs (DB calculated)</t>
+          <t>Epa Pah34</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>PAHs, total low molecular wt PAHs (reported)</t>
+          <t>Hpah1</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>CDFW-OSPR</t>
+          <t>Lpah1</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>EPA PAH16</t>
+          <t>Mn Pah13</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>EPA PAH34</t>
+          <t>Pah16</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>HPAH1</t>
+          <t>Pah44</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>LPAH1</t>
+          <t>Rbos Pah18</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>MN PAH13</t>
+          <t>Total_pah</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>PAH16</t>
+          <t>Wi_dnr Pah18</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>PAH44</t>
+          <t>Cross_tpah</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>RBOS PAH18</t>
+          <t>2,3,5-Trimethylnaphthalene</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>TOTAL_PAH</t>
+          <t>Benzo(E)Pyrene</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>WI_DNR PAH18</t>
+          <t>Pahs, Total For Washington State (17 Chems; Db Calc)</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>CROSS_TPAH</t>
+          <t>C3-Fluoranthenes/Pyrenes</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2,3,5-Trimethylnaphthalene</t>
+          <t>C4-Fluoranthenes/Pyrenes</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Benzo(e)pyrene</t>
+          <t>C4-Fluorene</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>PAHs, total for Washington State (17 chems; DB calc)</t>
+          <t>C2-Fluoranthenes/Pyrenes</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>C3-Fluoranthenes/pyrenes</t>
+          <t>Benzo[B]Thiophene</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>C4-Fluoranthenes/pyrenes</t>
+          <t>C1-Benzo[B]Thiophenes</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>C4-Fluorene</t>
+          <t>C1-Dibenzo(A,H)Anthracene</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>C2-Fluoranthenes/pyrenes</t>
+          <t>C1-Naphthobenzothiophenes</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Benzo(b)thiophene</t>
+          <t>C2-Benzo[B]Thiophenes</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>C1-Benzo(b)thiophenes</t>
+          <t>C2-Dibenzo(A,H)Anthracene</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>C1-Dibenzo(a,h)anthracene</t>
+          <t>C2-Naphthobenzothiophenes</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>C1-Naphthobenzothiophenes</t>
+          <t>C3-Benzo[B]Thiophenes</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>C2-Benzo(b)thiophenes</t>
+          <t>C3-Dibenzo(A,H)Anthracene</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>C2-Dibenzo(a,h)anthracene</t>
+          <t>C3-Naphthobenzothiophenes</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>C2-Naphthobenzothiophenes</t>
+          <t>Benzo(J+K)Fluoranthene</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>C3-Benzo(b)thiophenes</t>
+          <t>C4-Benzo[B]Thiophenes</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>C3-Dibenzo(a,h)anthracene</t>
+          <t>Chrysene + Triphenylene</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>C3-Naphthobenzothiophenes</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>Benzo(j+k)fluoranthene</t>
+          <t>Dibenzo(A,H+A,C)Anthracene</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>C4-Benzo(b)thiophenes</t>
+          <t>C-L Naphthalene</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Chrysene + Triphenylene</t>
+          <t>C-2 Naphthalene</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Dibenzo(a,h+a,c)anthracene</t>
+          <t>C-3 Naphthalene</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>C-4 Naphthalene</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>C-l Naphthalene</t>
+          <t>C-L Fluorene</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>C-2 Naphthalene</t>
+          <t>C-2 Fluorene</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>C-3 Naphthalene</t>
+          <t>C-3 Fluorene</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>C-4 Naphthalene</t>
+          <t>C-L Dibenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>C-l Fluorene</t>
+          <t>C-2 Dibenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>C-2 Fluorene</t>
+          <t>C-3 Dibenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>C-3 Fluorene</t>
+          <t>C-L Phenanthrene</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>C-l Dibenzothiophene</t>
+          <t>C-2 Phenanthrene</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>C-2 Dibenzothiophene</t>
+          <t>C-3 Phenanthrene</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>C-3 Dibenzothiophene</t>
+          <t>C-4 Phenanthrene</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>C-l Phenanthrene</t>
+          <t>C-L Pyrene</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>C-2 Phenanthrene</t>
+          <t>C-2 Pyrene</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>C-3 Phenanthrene</t>
+          <t>C-3 Pyrene</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>C-4 Phenanthrene</t>
+          <t>C-4 Pyrene</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>C-l Pyrene</t>
+          <t>Napthobenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>C-2 Pyrene</t>
+          <t>C-L Napthobenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>C-3 Pyrene</t>
+          <t>C-2 Napthobenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>C-4 Pyrene</t>
+          <t>C-3 Napthobenzothiophene</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Napthobenzothiophene</t>
+          <t>Benzo [A] Anthracene</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>C-l Napthobenzothiophene</t>
+          <t>C-L Chrysene</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>C-2 Napthobenzothiophene</t>
+          <t>C-2 Chrysene</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>C-3 Napthobenzothiophene</t>
+          <t>C-3 Chrysene</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Benzo (a) Anthracene</t>
+          <t>C-4 Chrysene</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>C-l Chrysene</t>
+          <t>Benzo [B] Fluoranthene</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>C-2 Chrysene</t>
+          <t>Benzo [K] Fluoranthene</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>C-3 Chrysene</t>
+          <t>Benzo [A] Pyrene</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>C-4 Chrysene</t>
+          <t>Indeno [1,2,3-C,D] Pyrene</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Benzo (b) Fluoranthene</t>
+          <t>Dibenzo (A,H)Anthracene</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Benzo (k) Fluoranthene</t>
+          <t>Benzo [G,H,I] Perylene</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Benzo (e) Pyrene</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>Benzo (a) Pyrene</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>Indeno (1,2,3 - cd) Pyrene</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>Dibenzo (a,h) Anthracene</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>Benzo (g,h,i) Perylene</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>TOTAL PAH</t>
+          <t>Total Pah</t>
         </is>
       </c>
     </row>

</xml_diff>